<commit_message>
all tests passing, some tests ignored. PHP7.4
</commit_message>
<xml_diff>
--- a/storage/framework/testing/TripsListTest.xlsx
+++ b/storage/framework/testing/TripsListTest.xlsx
@@ -70,6 +70,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2019-12-01T08:08:00</t>
     </r>
@@ -79,6 +80,7 @@
         <color rgb="FF808080"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.000Z</t>
     </r>
@@ -90,6 +92,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2019-12-01T09:09:00</t>
     </r>
@@ -99,6 +102,7 @@
         <color rgb="FF808080"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.000Z</t>
     </r>
@@ -110,6 +114,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2019-12-02T10:10:00</t>
     </r>
@@ -119,6 +124,7 @@
         <color rgb="FF808080"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.000Z</t>
     </r>
@@ -140,6 +146,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -161,12 +168,14 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -304,16 +313,16 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C21"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="29.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="29.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>